<commit_message>
change AppKey/NetworkKey and delete exist device
</commit_message>
<xml_diff>
--- a/chirpstack_deploy/nodelist.xlsx
+++ b/chirpstack_deploy/nodelist.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">70BED5FFFE010002</t>
   </si>
   <si>
-    <t xml:space="preserve"> 18201892d5cc45949e5110a38a6ed72e</t>
+    <t xml:space="preserve">18201892d5cc45949e5110a38a6ed72e</t>
   </si>
   <si>
     <t xml:space="preserve"> 48a9c8bb41e242e9b705f15f9288fe04</t>
@@ -785,7 +785,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -812,11 +812,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -861,7 +856,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -872,10 +867,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -902,7 +893,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -910,7 +901,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.75"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="74.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="74.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.2"/>
@@ -973,7 +964,7 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -999,7 +990,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="n">
@@ -1025,7 +1016,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="n">
@@ -1077,7 +1068,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="n">
@@ -1103,7 +1094,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1" t="n">
@@ -1129,7 +1120,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="n">
@@ -1178,7 +1169,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="n">
@@ -1201,7 +1192,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="n">
@@ -1224,7 +1215,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="n">
@@ -1273,7 +1264,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1" t="n">
@@ -1299,7 +1290,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="n">
@@ -1325,7 +1316,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="1" t="n">
@@ -1377,7 +1368,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="1" t="n">
@@ -1403,7 +1394,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="1" t="n">
@@ -1429,7 +1420,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="1" t="n">
@@ -1481,7 +1472,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="1" t="n">
@@ -1507,7 +1498,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="1" t="n">
@@ -1533,7 +1524,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="1" t="n">
@@ -1582,7 +1573,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="1" t="n">
@@ -1605,7 +1596,7 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="1" t="n">
@@ -1628,7 +1619,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B29" s="1" t="n">
@@ -1677,7 +1668,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B31" s="1" t="n">
@@ -1703,7 +1694,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B32" s="1" t="n">
@@ -1729,7 +1720,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B33" s="1" t="n">
@@ -1781,7 +1772,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B35" s="1" t="n">
@@ -1807,7 +1798,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B36" s="1" t="n">
@@ -1833,7 +1824,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="1" t="n">
@@ -1885,7 +1876,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B39" s="1" t="n">
@@ -1911,7 +1902,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B40" s="1" t="n">
@@ -1937,7 +1928,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B41" s="1" t="n">
@@ -1986,7 +1977,7 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B43" s="1" t="n">
@@ -2009,7 +2000,7 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B44" s="1" t="n">
@@ -2032,7 +2023,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="1" t="n">
@@ -2064,7 +2055,7 @@
       <c r="C46" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E46" s="0" t="s">
@@ -2081,7 +2072,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B47" s="1" t="n">
@@ -2090,7 +2081,7 @@
       <c r="C47" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E47" s="0" t="s">
@@ -2107,7 +2098,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B48" s="1" t="n">
@@ -2116,7 +2107,7 @@
       <c r="C48" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E48" s="0" t="s">
@@ -2133,7 +2124,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B49" s="1" t="n">

</xml_diff>